<commit_message>
Add an entry to the litterature review spreadsheet
Add to the spreadsheet the following reference: Luo, T., Cheng, Y., Falzon, J. et al. A framework to assess multi-hazard physical climate risk for power generation projects from publicly-accessible sources. Commun Earth Environ 4, 117 (2023). https://doi.org/10.1038/s43247-023-00782-w

Signed-off-by: EglantineGiraud <eglantine.giraud@gmail.com>
</commit_message>
<xml_diff>
--- a/methodology/literature/Literature_review.xlsx
+++ b/methodology/literature/Literature_review.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lsegroup-my.sharepoint.com/personal/claire_hugo_lseg_com/Documents/Documents/Physical Risks/Biblio/Working documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eglan\OneDrive\Documents\GitHub\physrisk\methodology\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC4F97D9-BAA1-4DA0-80DB-D6390FCE497F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0706C6C0-083C-45A5-8CF9-7C492524EE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{5E70EA40-22C4-4E82-B7B8-60E8844517C7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5E70EA40-22C4-4E82-B7B8-60E8844517C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Biblio" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Biblio!$A$2:$AH$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Biblio!$A$2:$AH$109</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="487">
   <si>
     <t>Authors</t>
   </si>
@@ -1485,13 +1485,28 @@
   </si>
   <si>
     <t>Damage functions by hazard/type of impact</t>
+  </si>
+  <si>
+    <t>Luo, T., Cheng, Y., Falzon, J. et al.</t>
+  </si>
+  <si>
+    <t>A framework to assess multi-hazard physical climate risk for power generation projects from publicly-accessible sources</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s43247-023-00782-w</t>
+  </si>
+  <si>
+    <t>Communications Earth &amp; Environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This article introduces a scalable and transparent methodology that enables multi-hazard physical climate risk assessments for any thermal or hydro power generation project. The methodology relies on basic power plant type and geolocation data inputs, publicly-available climate datasets, and hazard- and technology-specific vulnerability factors, to translate hazard severity into generation losses. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1659,32 +1674,11 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1713,48 +1707,6 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2096,32 +2048,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFBCA1A-30D0-406A-832D-88EB6CD9ED9E}">
-  <dimension ref="A1:AH108"/>
+  <dimension ref="A1:AH109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="I40" sqref="I40"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="2"/>
-    <col min="3" max="3" width="49.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" style="2" customWidth="1"/>
-    <col min="10" max="34" width="9.5703125" style="1" customWidth="1"/>
-    <col min="35" max="35" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="1" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="2"/>
+    <col min="3" max="3" width="49.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.453125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="21.1796875" style="2" customWidth="1"/>
+    <col min="10" max="34" width="9.54296875" style="1" customWidth="1"/>
+    <col min="35" max="35" width="6.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2181,7 +2133,7 @@
       <c r="AG1" s="19"/>
       <c r="AH1" s="19"/>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="J2" s="6" t="s">
         <v>12</v>
       </c>
@@ -2258,7 +2210,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="43.5">
+    <row r="3" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -2287,7 +2239,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="43.5">
+    <row r="4" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
@@ -2313,7 +2265,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="43.5">
+    <row r="5" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -2342,7 +2294,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="43.5">
+    <row r="6" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -2377,7 +2329,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="43.5">
+    <row r="7" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>59</v>
       </c>
@@ -2400,7 +2352,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="57.95">
+    <row r="8" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
@@ -2426,7 +2378,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="43.5">
+    <row r="9" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>67</v>
       </c>
@@ -2449,7 +2401,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="101.45">
+    <row r="10" spans="1:34" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>71</v>
       </c>
@@ -2478,7 +2430,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="43.5">
+    <row r="11" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>76</v>
       </c>
@@ -2519,7 +2471,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="29.1">
+    <row r="12" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>82</v>
       </c>
@@ -2545,7 +2497,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="43.5">
+    <row r="13" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>87</v>
       </c>
@@ -2571,7 +2523,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="43.5">
+    <row r="14" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>91</v>
       </c>
@@ -2606,7 +2558,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="29.1">
+    <row r="15" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>97</v>
       </c>
@@ -2629,7 +2581,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="43.5">
+    <row r="16" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>101</v>
       </c>
@@ -2656,7 +2608,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="43.5">
+    <row r="17" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>106</v>
       </c>
@@ -2677,7 +2629,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="57.95">
+    <row r="18" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>106</v>
       </c>
@@ -2709,7 +2661,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="57.95">
+    <row r="19" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>114</v>
       </c>
@@ -2750,7 +2702,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="43.5">
+    <row r="20" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>119</v>
       </c>
@@ -2770,7 +2722,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:33" ht="57.95">
+    <row r="21" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>123</v>
       </c>
@@ -2796,7 +2748,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="87">
+    <row r="22" spans="1:33" ht="87" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>127</v>
       </c>
@@ -2816,7 +2768,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="43.5">
+    <row r="23" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>130</v>
       </c>
@@ -2839,7 +2791,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="72.599999999999994">
+    <row r="24" spans="1:33" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>134</v>
       </c>
@@ -2862,7 +2814,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="43.5">
+    <row r="25" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>139</v>
       </c>
@@ -2888,7 +2840,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="57.95">
+    <row r="26" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>144</v>
       </c>
@@ -2920,7 +2872,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="48.95" customHeight="1">
+    <row r="27" spans="1:33" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>149</v>
       </c>
@@ -2946,7 +2898,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="72.599999999999994">
+    <row r="28" spans="1:33" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>153</v>
       </c>
@@ -2972,7 +2924,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="57.95">
+    <row r="29" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>158</v>
       </c>
@@ -2995,7 +2947,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:33" ht="87">
+    <row r="30" spans="1:33" ht="87" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>162</v>
       </c>
@@ -3018,7 +2970,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:33" ht="43.5">
+    <row r="31" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>165</v>
       </c>
@@ -3038,7 +2990,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:33" ht="144.94999999999999">
+    <row r="32" spans="1:33" ht="145" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>169</v>
       </c>
@@ -3073,7 +3025,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="29.1">
+    <row r="33" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>174</v>
       </c>
@@ -3108,7 +3060,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="57.95">
+    <row r="34" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>180</v>
       </c>
@@ -3170,7 +3122,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="72.599999999999994">
+    <row r="35" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>184</v>
       </c>
@@ -3205,7 +3157,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="43.5">
+    <row r="36" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>188</v>
       </c>
@@ -3237,7 +3189,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="43.5">
+    <row r="37" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>195</v>
       </c>
@@ -3269,7 +3221,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="57.95">
+    <row r="38" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>200</v>
       </c>
@@ -3298,7 +3250,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="29.1">
+    <row r="39" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>204</v>
       </c>
@@ -3321,7 +3273,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="43.5">
+    <row r="40" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>208</v>
       </c>
@@ -3347,7 +3299,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="57.95">
+    <row r="41" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>212</v>
       </c>
@@ -3373,7 +3325,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="57.95">
+    <row r="42" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>216</v>
       </c>
@@ -3408,7 +3360,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:34" ht="43.5">
+    <row r="43" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>221</v>
       </c>
@@ -3428,7 +3380,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:34" ht="43.5">
+    <row r="44" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>224</v>
       </c>
@@ -3460,7 +3412,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:34" ht="43.5">
+    <row r="45" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>224</v>
       </c>
@@ -3492,7 +3444,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:34" ht="43.5">
+    <row r="46" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>232</v>
       </c>
@@ -3512,7 +3464,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:34" ht="57.95">
+    <row r="47" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>236</v>
       </c>
@@ -3550,7 +3502,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:34" ht="43.5">
+    <row r="48" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>240</v>
       </c>
@@ -3582,7 +3534,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:34" ht="43.5">
+    <row r="49" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>246</v>
       </c>
@@ -3617,7 +3569,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:34" ht="144.94999999999999">
+    <row r="50" spans="1:34" ht="145" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>251</v>
       </c>
@@ -3643,7 +3595,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:34" ht="43.5">
+    <row r="51" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>256</v>
       </c>
@@ -3669,7 +3621,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:34" ht="101.45">
+    <row r="52" spans="1:34" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>260</v>
       </c>
@@ -3689,7 +3641,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:34" ht="87">
+    <row r="53" spans="1:34" ht="87" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>264</v>
       </c>
@@ -3712,7 +3664,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:34" ht="29.1">
+    <row r="54" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>268</v>
       </c>
@@ -3750,7 +3702,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:34" ht="43.5">
+    <row r="55" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>273</v>
       </c>
@@ -3777,7 +3729,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:34" ht="29.1">
+    <row r="56" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>278</v>
       </c>
@@ -3803,7 +3755,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:34" ht="144.94999999999999">
+    <row r="57" spans="1:34" ht="145" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>284</v>
       </c>
@@ -3829,7 +3781,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:34" ht="43.5">
+    <row r="58" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>288</v>
       </c>
@@ -3855,7 +3807,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:34" ht="72.599999999999994">
+    <row r="59" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>288</v>
       </c>
@@ -3881,7 +3833,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:34" ht="29.1">
+    <row r="60" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>295</v>
       </c>
@@ -3907,7 +3859,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:34" ht="72.599999999999994">
+    <row r="61" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>298</v>
       </c>
@@ -3927,7 +3879,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:34" ht="57.95">
+    <row r="62" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>302</v>
       </c>
@@ -3962,7 +3914,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:34" ht="43.5">
+    <row r="63" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>308</v>
       </c>
@@ -3985,7 +3937,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:34" ht="43.5">
+    <row r="64" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>311</v>
       </c>
@@ -4008,7 +3960,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:34" ht="57.95">
+    <row r="65" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>314</v>
       </c>
@@ -4028,7 +3980,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="1:34" ht="43.5">
+    <row r="66" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>314</v>
       </c>
@@ -4066,7 +4018,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:34" ht="43.5">
+    <row r="67" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>314</v>
       </c>
@@ -4092,7 +4044,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:34" ht="43.5">
+    <row r="68" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>324</v>
       </c>
@@ -4130,7 +4082,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="1:34" ht="43.5">
+    <row r="69" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>327</v>
       </c>
@@ -4156,7 +4108,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="70" spans="1:34" ht="101.45">
+    <row r="70" spans="1:34" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>330</v>
       </c>
@@ -4188,7 +4140,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="1:34" ht="57.95">
+    <row r="71" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>335</v>
       </c>
@@ -4211,7 +4163,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="72" spans="1:34" ht="57.95">
+    <row r="72" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>339</v>
       </c>
@@ -4231,7 +4183,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="73" spans="1:34" ht="43.5">
+    <row r="73" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>342</v>
       </c>
@@ -4251,7 +4203,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:34" ht="43.5">
+    <row r="74" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>346</v>
       </c>
@@ -4271,7 +4223,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:34" ht="72.599999999999994">
+    <row r="75" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>350</v>
       </c>
@@ -4303,7 +4255,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="1:34" ht="87">
+    <row r="76" spans="1:34" ht="87" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>355</v>
       </c>
@@ -4329,7 +4281,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="77" spans="1:34" ht="43.5">
+    <row r="77" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>358</v>
       </c>
@@ -4364,7 +4316,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="78" spans="1:34" ht="43.5">
+    <row r="78" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>362</v>
       </c>
@@ -4387,7 +4339,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:34" ht="116.1">
+    <row r="79" spans="1:34" ht="116" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>365</v>
       </c>
@@ -4425,7 +4377,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="80" spans="1:34" ht="29.1">
+    <row r="80" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>371</v>
       </c>
@@ -4451,7 +4403,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="81" spans="1:33" ht="57.95">
+    <row r="81" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>375</v>
       </c>
@@ -4474,7 +4426,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="82" spans="1:33" ht="29.1">
+    <row r="82" spans="1:33" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>378</v>
       </c>
@@ -4494,7 +4446,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:33" ht="29.1">
+    <row r="83" spans="1:33" ht="29" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>382</v>
       </c>
@@ -4529,7 +4481,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:33" ht="130.5">
+    <row r="84" spans="1:33" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>386</v>
       </c>
@@ -4552,7 +4504,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="85" spans="1:33" ht="43.5">
+    <row r="85" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>391</v>
       </c>
@@ -4578,7 +4530,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="86" spans="1:33" ht="43.5">
+    <row r="86" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>395</v>
       </c>
@@ -4598,7 +4550,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="87" spans="1:33" ht="43.5">
+    <row r="87" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>399</v>
       </c>
@@ -4618,7 +4570,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="88" spans="1:33" ht="43.5">
+    <row r="88" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>402</v>
       </c>
@@ -4641,7 +4593,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="89" spans="1:33" ht="43.5">
+    <row r="89" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>405</v>
       </c>
@@ -4661,7 +4613,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="90" spans="1:33" ht="116.1">
+    <row r="90" spans="1:33" ht="116" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>409</v>
       </c>
@@ -4681,7 +4633,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="91" spans="1:33" ht="43.5">
+    <row r="91" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>413</v>
       </c>
@@ -4701,7 +4653,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="92" spans="1:33" ht="72.599999999999994">
+    <row r="92" spans="1:33" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>417</v>
       </c>
@@ -4724,7 +4676,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="93" spans="1:33" ht="43.5">
+    <row r="93" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>421</v>
       </c>
@@ -4747,7 +4699,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="94" spans="1:33" ht="43.5">
+    <row r="94" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>426</v>
       </c>
@@ -4770,7 +4722,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="95" spans="1:33" ht="130.5">
+    <row r="95" spans="1:33" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>430</v>
       </c>
@@ -4802,7 +4754,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="96" spans="1:33" ht="43.5">
+    <row r="96" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>434</v>
       </c>
@@ -4822,7 +4774,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="97" spans="1:34" ht="43.5">
+    <row r="97" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>438</v>
       </c>
@@ -4845,7 +4797,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="98" spans="1:34" ht="43.5">
+    <row r="98" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>442</v>
       </c>
@@ -4883,318 +4835,356 @@
         <v>43</v>
       </c>
     </row>
-    <row r="99" spans="1:34" ht="43.5">
+    <row r="99" spans="1:34" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B99" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="E99" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N99" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R99" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S99" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH99" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="100" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A100" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="B99" s="9">
+      <c r="B100" s="9">
         <v>2018</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="D99" s="11" t="s">
+      <c r="D100" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E99" s="14" t="s">
+      <c r="E100" s="14" t="s">
         <v>449</v>
       </c>
-      <c r="F99" s="2" t="s">
+      <c r="F100" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G99" s="2" t="s">
+      <c r="G100" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K99" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG99" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="100" spans="1:34" ht="29.1">
-      <c r="A100" s="2" t="s">
+      <c r="K100" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG100" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="101" spans="1:34" ht="29" x14ac:dyDescent="0.35">
+      <c r="A101" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B100" s="3">
+      <c r="B101" s="3">
         <v>2018</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="D100" s="11" t="s">
+      <c r="D101" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E100" s="14" t="s">
+      <c r="E101" s="14" t="s">
         <v>452</v>
       </c>
-      <c r="K100" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O100" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="101" spans="1:34" ht="57.95">
-      <c r="A101" s="2" t="s">
+      <c r="K101" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O101" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="102" spans="1:34" ht="58" x14ac:dyDescent="0.35">
+      <c r="A102" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B102" s="2">
         <v>2017</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="D101" s="11" t="s">
+      <c r="D102" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E101" s="14" t="s">
+      <c r="E102" s="14" t="s">
         <v>455</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F102" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N101" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R101" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="102" spans="1:34" ht="87">
-      <c r="A102" s="2" t="s">
+      <c r="N102" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R102" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="103" spans="1:34" ht="87" x14ac:dyDescent="0.35">
+      <c r="A103" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="B102" s="2">
+      <c r="B103" s="2">
         <v>2020</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="D102" s="11" t="s">
+      <c r="D103" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="E102" s="14" t="s">
+      <c r="E103" s="14" t="s">
         <v>459</v>
       </c>
-      <c r="F102" s="2" t="s">
+      <c r="F103" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="H102" s="10" t="s">
+      <c r="H103" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I102" s="2" t="s">
+      <c r="I103" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="N102" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z102" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="103" spans="1:34" ht="29.1">
-      <c r="A103" s="2" t="s">
+      <c r="N103" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z103" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="104" spans="1:34" ht="29" x14ac:dyDescent="0.35">
+      <c r="A104" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="B103" s="3">
+      <c r="B104" s="3">
         <v>2020</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C104" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="D103" s="11" t="s">
+      <c r="D104" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="E103" s="14" t="s">
+      <c r="E104" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="F103" s="2" t="s">
+      <c r="F104" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K103" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="104" spans="1:34" ht="57.95">
-      <c r="A104" s="2" t="s">
+      <c r="K104" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="105" spans="1:34" ht="58" x14ac:dyDescent="0.35">
+      <c r="A105" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="B104" s="2">
+      <c r="B105" s="2">
         <v>2004</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C105" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="D104" s="11" t="s">
+      <c r="D105" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="E104" s="14" t="s">
+      <c r="E105" s="14" t="s">
         <v>466</v>
       </c>
-      <c r="H104" s="10" t="s">
+      <c r="H105" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I104" s="2" t="s">
+      <c r="I105" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="K104" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M104" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="105" spans="1:34" ht="43.5">
-      <c r="A105" s="2" t="s">
+      <c r="K105" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M105" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="106" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A106" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="B105" s="3">
-        <v>2021</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="D105" s="11" t="s">
-        <v>470</v>
-      </c>
-      <c r="E105" s="14" t="s">
-        <v>471</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J105" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE105" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="106" spans="1:34" ht="43.5">
-      <c r="A106" s="2" t="s">
-        <v>472</v>
       </c>
       <c r="B106" s="3">
         <v>2021</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D106" s="11" t="s">
         <v>470</v>
       </c>
       <c r="E106" s="14" t="s">
-        <v>474</v>
+        <v>471</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="J106" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="T106" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC106" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="107" spans="1:34" ht="57.95">
+      <c r="AE106" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="107" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="B107" s="2">
+      <c r="B107" s="3">
+        <v>2021</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="D107" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="E107" s="14" t="s">
+        <v>474</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T107" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC107" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="108" spans="1:34" ht="58" x14ac:dyDescent="0.35">
+      <c r="A108" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B108" s="2">
         <v>2017</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="D107" s="11" t="s">
+      <c r="D108" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E107" s="16" t="s">
+      <c r="E108" s="16" t="s">
         <v>476</v>
       </c>
-      <c r="N107" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O107" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH107" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="108" spans="1:34" ht="72.599999999999994">
-      <c r="A108" s="2" t="s">
+      <c r="N108" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O108" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH108" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="109" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A109" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="B108" s="2">
+      <c r="B109" s="2">
         <v>2021</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C109" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="D108" s="11" t="s">
+      <c r="D109" s="11" t="s">
         <v>479</v>
       </c>
-      <c r="E108" s="14" t="s">
+      <c r="E109" s="14" t="s">
         <v>480</v>
       </c>
-      <c r="F108" s="2" t="s">
+      <c r="F109" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G108" s="2" t="s">
+      <c r="G109" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="H108" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="I108" s="2" t="s">
+      <c r="H109" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I109" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH108" s="1" t="s">
+      <c r="J109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH109" s="1" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AH108" xr:uid="{2CFBCA1A-30D0-406A-832D-88EB6CD9ED9E}">
+  <autoFilter ref="A2:AH109" xr:uid="{2CFBCA1A-30D0-406A-832D-88EB6CD9ED9E}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AH83">
       <sortCondition ref="A3:A83"/>
       <sortCondition descending="1" ref="B3:B83"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AH108">
-    <sortCondition ref="A3:A108"/>
-    <sortCondition descending="1" ref="B3:B108"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AH109">
+    <sortCondition ref="A3:A109"/>
+    <sortCondition descending="1" ref="B3:B109"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="J1:N1"/>
@@ -5202,70 +5192,37 @@
     <mergeCell ref="AC1:AH1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H106 H109:H1048576 H56:H104 H1:H54">
-    <cfRule type="containsText" dxfId="17" priority="27" operator="containsText" text="tbc">
+  <conditionalFormatting sqref="H1:H54">
+    <cfRule type="containsText" dxfId="8" priority="27" operator="containsText" text="tbc">
       <formula>NOT(ISERROR(SEARCH("tbc",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="42" operator="containsText" text="to see">
+    <cfRule type="containsText" dxfId="7" priority="42" operator="containsText" text="to see">
       <formula>NOT(ISERROR(SEARCH("to see",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="43" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="6" priority="43" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="44" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="5" priority="44" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI3:AI89">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="pb">
-      <formula>NOT(ISERROR(SEARCH("pb",AI3)))</formula>
+  <conditionalFormatting sqref="H56:H1048576">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="tbc">
+      <formula>NOT(ISERROR(SEARCH("tbc",H56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="to see">
+      <formula>NOT(ISERROR(SEARCH("to see",H56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",H56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",H56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI90:AI99">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="pb">
-      <formula>NOT(ISERROR(SEARCH("pb",AI90)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H105">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="tbc">
-      <formula>NOT(ISERROR(SEARCH("tbc",H105)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="to see">
-      <formula>NOT(ISERROR(SEARCH("to see",H105)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",H105)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",H105)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H107">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="tbc">
-      <formula>NOT(ISERROR(SEARCH("tbc",H107)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="to see">
-      <formula>NOT(ISERROR(SEARCH("to see",H107)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",H107)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",H107)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H108">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="tbc">
-      <formula>NOT(ISERROR(SEARCH("tbc",H108)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="to see">
-      <formula>NOT(ISERROR(SEARCH("to see",H108)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",H108)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",H108)))</formula>
+  <conditionalFormatting sqref="AI3:AI100">
+    <cfRule type="containsText" dxfId="0" priority="13" operator="containsText" text="pb">
+      <formula>NOT(ISERROR(SEARCH("pb",AI3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -5278,14 +5235,14 @@
     <hyperlink ref="E62" r:id="rId7" xr:uid="{027C1889-F71D-41F9-AAB3-710415514B9A}"/>
     <hyperlink ref="E64" r:id="rId8" xr:uid="{7F16FD1B-410C-4736-B12B-538ED1B1CA4A}"/>
     <hyperlink ref="E73" r:id="rId9" xr:uid="{96547B7D-03C7-4FB0-871E-52924B32F313}"/>
-    <hyperlink ref="E100" r:id="rId10" xr:uid="{669A4DC3-F305-4158-821E-9DDF7FA031D9}"/>
+    <hyperlink ref="E101" r:id="rId10" xr:uid="{669A4DC3-F305-4158-821E-9DDF7FA031D9}"/>
     <hyperlink ref="E74" r:id="rId11" xr:uid="{494A117E-C8A0-4172-AB2B-CBDB4AD3EB9C}"/>
     <hyperlink ref="E63" r:id="rId12" xr:uid="{099984D8-6082-40F0-9E84-E49E1BB5574C}"/>
     <hyperlink ref="E43" r:id="rId13" xr:uid="{BE14CD70-8EAE-48EB-8DBB-26D14DD3169E}"/>
     <hyperlink ref="E91" r:id="rId14" xr:uid="{E6E9C87F-4F38-4FB1-B153-C74AAFDF2F2B}"/>
     <hyperlink ref="E85" r:id="rId15" xr:uid="{E400C837-FFD8-481F-B368-EE894FCDA1BC}"/>
     <hyperlink ref="E87" r:id="rId16" xr:uid="{2DA9E77C-A279-407D-A22A-DBB8036D095C}"/>
-    <hyperlink ref="E103" r:id="rId17" xr:uid="{4B54B9BB-8F33-47B5-A90B-B10DB08E0813}"/>
+    <hyperlink ref="E104" r:id="rId17" xr:uid="{4B54B9BB-8F33-47B5-A90B-B10DB08E0813}"/>
     <hyperlink ref="E7" r:id="rId18" xr:uid="{95E7CD7F-AF88-45EC-8F37-E5E9D1EF1034}"/>
     <hyperlink ref="E17" r:id="rId19" xr:uid="{E0EBEC91-B437-46E7-825D-8215BE6C2171}"/>
     <hyperlink ref="E31" r:id="rId20" xr:uid="{112A3FCC-C815-4772-8173-B88F7D873D08}"/>
@@ -5312,7 +5269,7 @@
     <hyperlink ref="E21" r:id="rId41" xr:uid="{C0C54509-B25E-4A61-A33B-9BC669C139B1}"/>
     <hyperlink ref="E24" r:id="rId42" xr:uid="{17CBDD15-89FB-4714-8293-10AA629C94AE}"/>
     <hyperlink ref="E25" r:id="rId43" xr:uid="{56704F90-1A3C-477A-B777-D214530F6C5F}"/>
-    <hyperlink ref="E108" r:id="rId44" xr:uid="{911F88E0-33FE-4735-A223-7A0A51988D6C}"/>
+    <hyperlink ref="E109" r:id="rId44" xr:uid="{911F88E0-33FE-4735-A223-7A0A51988D6C}"/>
     <hyperlink ref="E30" r:id="rId45" location=":~:text=Both%20scenarios%20show%20that%2C%20at,)%2C%20while%20nuclear%20power%20decreases." xr:uid="{EA05B2F9-69A3-4830-B3AD-7E1B7CE631D1}"/>
     <hyperlink ref="E35" r:id="rId46" xr:uid="{25B0BDC6-0A3E-48D3-A3E8-32E6F3075DCC}"/>
     <hyperlink ref="E36" r:id="rId47" xr:uid="{67A7E60B-B849-4080-A8A3-0BBA26FED531}"/>
@@ -5344,11 +5301,11 @@
     <hyperlink ref="E95" r:id="rId73" location=":~:text=Windstorms%20are%20amongst%20the%20most,annual%20losses%20in%20the%20EU.&amp;text=As%20a%20consequence%2C%20it%20is,rise%20due%20to%20climate%20change." xr:uid="{84766123-8B9C-40D7-9092-EE32EC59F2D3}"/>
     <hyperlink ref="E97" r:id="rId74" xr:uid="{EE1C6824-4127-49BF-856B-54D15A26EEC3}"/>
     <hyperlink ref="E27" r:id="rId75" xr:uid="{8772BA96-ED44-4481-A6D6-CAB4C1D2D36D}"/>
-    <hyperlink ref="E99" r:id="rId76" xr:uid="{A8B1A50A-41B3-4028-8B6D-55BA1E74EF06}"/>
+    <hyperlink ref="E100" r:id="rId76" xr:uid="{A8B1A50A-41B3-4028-8B6D-55BA1E74EF06}"/>
     <hyperlink ref="E70" r:id="rId77" xr:uid="{7A6C35C0-065D-48C9-81B5-5BAC2E227370}"/>
-    <hyperlink ref="E105" r:id="rId78" xr:uid="{18FEDC5F-D897-4BD3-B5F5-B23D6192D5C7}"/>
-    <hyperlink ref="E106" r:id="rId79" xr:uid="{188633F7-D468-4FF1-B629-6E1DEC4631EE}"/>
-    <hyperlink ref="E107" r:id="rId80" xr:uid="{6FAF70A0-3FCF-454F-9682-BAB8A8C9D3E7}"/>
+    <hyperlink ref="E106" r:id="rId78" xr:uid="{18FEDC5F-D897-4BD3-B5F5-B23D6192D5C7}"/>
+    <hyperlink ref="E107" r:id="rId79" xr:uid="{188633F7-D468-4FF1-B629-6E1DEC4631EE}"/>
+    <hyperlink ref="E108" r:id="rId80" xr:uid="{6FAF70A0-3FCF-454F-9682-BAB8A8C9D3E7}"/>
     <hyperlink ref="E79" r:id="rId81" xr:uid="{D9A56F1D-2229-42A5-84AC-9DA4A78FF246}"/>
     <hyperlink ref="E42" r:id="rId82" xr:uid="{44C7D96C-57CD-4E32-B593-A7F8B9769E84}"/>
     <hyperlink ref="E54" r:id="rId83" xr:uid="{961F3F75-E073-4BB0-A98B-0BE784E6D0A8}"/>
@@ -5359,24 +5316,25 @@
     <hyperlink ref="E50" r:id="rId88" xr:uid="{88DFAFA3-C726-468A-934C-491527C128D6}"/>
     <hyperlink ref="E48" r:id="rId89" xr:uid="{F591CC07-7435-4E15-9D93-39528ACCE89B}"/>
     <hyperlink ref="E75" r:id="rId90" xr:uid="{ED87634C-0B58-4EAF-BEDB-2A48A969155C}"/>
-    <hyperlink ref="E104" r:id="rId91" xr:uid="{C77ED42E-2BAE-4561-B014-7D5CCCD7300B}"/>
+    <hyperlink ref="E105" r:id="rId91" xr:uid="{C77ED42E-2BAE-4561-B014-7D5CCCD7300B}"/>
     <hyperlink ref="E52" r:id="rId92" xr:uid="{AE60E41F-78E6-4C0B-99CC-9B9F011A14D2}"/>
     <hyperlink ref="E22" r:id="rId93" xr:uid="{D2CDFB65-960D-4324-9309-D75DB0AE6DE1}"/>
     <hyperlink ref="E32" r:id="rId94" xr:uid="{78010408-7D00-4480-9D3C-B780BB49E81D}"/>
     <hyperlink ref="E8" r:id="rId95" xr:uid="{2220BCD0-A5B0-4A1D-AA6D-A1D41EBDE3CE}"/>
-    <hyperlink ref="E101" r:id="rId96" xr:uid="{3338E87A-5ECB-4F9B-ACE2-2EC0716ABFED}"/>
+    <hyperlink ref="E102" r:id="rId96" xr:uid="{3338E87A-5ECB-4F9B-ACE2-2EC0716ABFED}"/>
     <hyperlink ref="E80" r:id="rId97" xr:uid="{C18AFA26-2EB1-499D-B2B4-72BB9C037E10}"/>
     <hyperlink ref="E26" r:id="rId98" xr:uid="{7D25A591-E8A8-418A-A32D-CDEB86ABCE99}"/>
     <hyperlink ref="E28" r:id="rId99" xr:uid="{2582EDBD-D337-4487-BD2B-35A6BA106688}"/>
     <hyperlink ref="E76" r:id="rId100" xr:uid="{93645E69-F230-4737-B909-AF6297441E90}"/>
     <hyperlink ref="E57" r:id="rId101" xr:uid="{A4270E10-FA55-4CD6-89BD-993EB73F11ED}"/>
     <hyperlink ref="E33" r:id="rId102" xr:uid="{7C482A88-1330-4A10-AE85-2F21D5F0D01B}"/>
-    <hyperlink ref="E102" r:id="rId103" xr:uid="{82E79761-A535-494D-98AA-10AEED4B01D5}"/>
+    <hyperlink ref="E103" r:id="rId103" xr:uid="{82E79761-A535-494D-98AA-10AEED4B01D5}"/>
     <hyperlink ref="E58" r:id="rId104" xr:uid="{74A01E59-FEDC-471C-A936-DCE757B765DE}"/>
     <hyperlink ref="E77" r:id="rId105" xr:uid="{C16C0228-218F-4349-9E17-C55FCC0E4848}"/>
     <hyperlink ref="E83" r:id="rId106" xr:uid="{16CF4C79-2C66-473B-8376-0E52D53979DE}"/>
+    <hyperlink ref="E99" r:id="rId107" xr:uid="{6B3A7836-3287-4B71-BAE9-EBE88E438E91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId107"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId108"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add an entry to the litterature review spreadsheet (#246)
Add to the spreadsheet the following reference: Luo, T., Cheng, Y., Falzon, J. et al. A framework to assess multi-hazard physical climate risk for power generation projects from publicly-accessible sources. Commun Earth Environ 4, 117 (2023). https://doi.org/10.1038/s43247-023-00782-w

Signed-off-by: EglantineGiraud <eglantine.giraud@gmail.com>
</commit_message>
<xml_diff>
--- a/methodology/literature/Literature_review.xlsx
+++ b/methodology/literature/Literature_review.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lsegroup-my.sharepoint.com/personal/claire_hugo_lseg_com/Documents/Documents/Physical Risks/Biblio/Working documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eglan\OneDrive\Documents\GitHub\physrisk\methodology\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC4F97D9-BAA1-4DA0-80DB-D6390FCE497F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0706C6C0-083C-45A5-8CF9-7C492524EE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{5E70EA40-22C4-4E82-B7B8-60E8844517C7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5E70EA40-22C4-4E82-B7B8-60E8844517C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Biblio" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Biblio!$A$2:$AH$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Biblio!$A$2:$AH$109</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="487">
   <si>
     <t>Authors</t>
   </si>
@@ -1485,13 +1485,28 @@
   </si>
   <si>
     <t>Damage functions by hazard/type of impact</t>
+  </si>
+  <si>
+    <t>Luo, T., Cheng, Y., Falzon, J. et al.</t>
+  </si>
+  <si>
+    <t>A framework to assess multi-hazard physical climate risk for power generation projects from publicly-accessible sources</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s43247-023-00782-w</t>
+  </si>
+  <si>
+    <t>Communications Earth &amp; Environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This article introduces a scalable and transparent methodology that enables multi-hazard physical climate risk assessments for any thermal or hydro power generation project. The methodology relies on basic power plant type and geolocation data inputs, publicly-available climate datasets, and hazard- and technology-specific vulnerability factors, to translate hazard severity into generation losses. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1659,32 +1674,11 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1713,48 +1707,6 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2096,32 +2048,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFBCA1A-30D0-406A-832D-88EB6CD9ED9E}">
-  <dimension ref="A1:AH108"/>
+  <dimension ref="A1:AH109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="I40" sqref="I40"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="2"/>
-    <col min="3" max="3" width="49.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" style="2" customWidth="1"/>
-    <col min="10" max="34" width="9.5703125" style="1" customWidth="1"/>
-    <col min="35" max="35" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="1" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="2"/>
+    <col min="3" max="3" width="49.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.453125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="21.1796875" style="2" customWidth="1"/>
+    <col min="10" max="34" width="9.54296875" style="1" customWidth="1"/>
+    <col min="35" max="35" width="6.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2181,7 +2133,7 @@
       <c r="AG1" s="19"/>
       <c r="AH1" s="19"/>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="J2" s="6" t="s">
         <v>12</v>
       </c>
@@ -2258,7 +2210,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="43.5">
+    <row r="3" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -2287,7 +2239,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="43.5">
+    <row r="4" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
@@ -2313,7 +2265,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="43.5">
+    <row r="5" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -2342,7 +2294,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="43.5">
+    <row r="6" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -2377,7 +2329,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="43.5">
+    <row r="7" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>59</v>
       </c>
@@ -2400,7 +2352,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="57.95">
+    <row r="8" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
@@ -2426,7 +2378,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="43.5">
+    <row r="9" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>67</v>
       </c>
@@ -2449,7 +2401,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="101.45">
+    <row r="10" spans="1:34" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>71</v>
       </c>
@@ -2478,7 +2430,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="43.5">
+    <row r="11" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>76</v>
       </c>
@@ -2519,7 +2471,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="29.1">
+    <row r="12" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>82</v>
       </c>
@@ -2545,7 +2497,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="43.5">
+    <row r="13" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>87</v>
       </c>
@@ -2571,7 +2523,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="43.5">
+    <row r="14" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>91</v>
       </c>
@@ -2606,7 +2558,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="29.1">
+    <row r="15" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>97</v>
       </c>
@@ -2629,7 +2581,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="43.5">
+    <row r="16" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>101</v>
       </c>
@@ -2656,7 +2608,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="43.5">
+    <row r="17" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>106</v>
       </c>
@@ -2677,7 +2629,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="57.95">
+    <row r="18" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>106</v>
       </c>
@@ -2709,7 +2661,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="57.95">
+    <row r="19" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>114</v>
       </c>
@@ -2750,7 +2702,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="43.5">
+    <row r="20" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>119</v>
       </c>
@@ -2770,7 +2722,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:33" ht="57.95">
+    <row r="21" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>123</v>
       </c>
@@ -2796,7 +2748,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="87">
+    <row r="22" spans="1:33" ht="87" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>127</v>
       </c>
@@ -2816,7 +2768,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="43.5">
+    <row r="23" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>130</v>
       </c>
@@ -2839,7 +2791,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="72.599999999999994">
+    <row r="24" spans="1:33" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>134</v>
       </c>
@@ -2862,7 +2814,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="43.5">
+    <row r="25" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>139</v>
       </c>
@@ -2888,7 +2840,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="57.95">
+    <row r="26" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>144</v>
       </c>
@@ -2920,7 +2872,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="48.95" customHeight="1">
+    <row r="27" spans="1:33" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>149</v>
       </c>
@@ -2946,7 +2898,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="72.599999999999994">
+    <row r="28" spans="1:33" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>153</v>
       </c>
@@ -2972,7 +2924,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="57.95">
+    <row r="29" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>158</v>
       </c>
@@ -2995,7 +2947,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:33" ht="87">
+    <row r="30" spans="1:33" ht="87" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>162</v>
       </c>
@@ -3018,7 +2970,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:33" ht="43.5">
+    <row r="31" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>165</v>
       </c>
@@ -3038,7 +2990,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:33" ht="144.94999999999999">
+    <row r="32" spans="1:33" ht="145" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>169</v>
       </c>
@@ -3073,7 +3025,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="29.1">
+    <row r="33" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>174</v>
       </c>
@@ -3108,7 +3060,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="57.95">
+    <row r="34" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>180</v>
       </c>
@@ -3170,7 +3122,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="72.599999999999994">
+    <row r="35" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>184</v>
       </c>
@@ -3205,7 +3157,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="43.5">
+    <row r="36" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>188</v>
       </c>
@@ -3237,7 +3189,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="43.5">
+    <row r="37" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>195</v>
       </c>
@@ -3269,7 +3221,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="57.95">
+    <row r="38" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>200</v>
       </c>
@@ -3298,7 +3250,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="29.1">
+    <row r="39" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>204</v>
       </c>
@@ -3321,7 +3273,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="43.5">
+    <row r="40" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>208</v>
       </c>
@@ -3347,7 +3299,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="57.95">
+    <row r="41" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>212</v>
       </c>
@@ -3373,7 +3325,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="57.95">
+    <row r="42" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>216</v>
       </c>
@@ -3408,7 +3360,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:34" ht="43.5">
+    <row r="43" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>221</v>
       </c>
@@ -3428,7 +3380,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:34" ht="43.5">
+    <row r="44" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>224</v>
       </c>
@@ -3460,7 +3412,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:34" ht="43.5">
+    <row r="45" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>224</v>
       </c>
@@ -3492,7 +3444,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:34" ht="43.5">
+    <row r="46" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>232</v>
       </c>
@@ -3512,7 +3464,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:34" ht="57.95">
+    <row r="47" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>236</v>
       </c>
@@ -3550,7 +3502,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:34" ht="43.5">
+    <row r="48" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>240</v>
       </c>
@@ -3582,7 +3534,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:34" ht="43.5">
+    <row r="49" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>246</v>
       </c>
@@ -3617,7 +3569,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:34" ht="144.94999999999999">
+    <row r="50" spans="1:34" ht="145" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>251</v>
       </c>
@@ -3643,7 +3595,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:34" ht="43.5">
+    <row r="51" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>256</v>
       </c>
@@ -3669,7 +3621,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:34" ht="101.45">
+    <row r="52" spans="1:34" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>260</v>
       </c>
@@ -3689,7 +3641,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:34" ht="87">
+    <row r="53" spans="1:34" ht="87" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>264</v>
       </c>
@@ -3712,7 +3664,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:34" ht="29.1">
+    <row r="54" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>268</v>
       </c>
@@ -3750,7 +3702,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:34" ht="43.5">
+    <row r="55" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>273</v>
       </c>
@@ -3777,7 +3729,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:34" ht="29.1">
+    <row r="56" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>278</v>
       </c>
@@ -3803,7 +3755,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:34" ht="144.94999999999999">
+    <row r="57" spans="1:34" ht="145" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>284</v>
       </c>
@@ -3829,7 +3781,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:34" ht="43.5">
+    <row r="58" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>288</v>
       </c>
@@ -3855,7 +3807,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:34" ht="72.599999999999994">
+    <row r="59" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>288</v>
       </c>
@@ -3881,7 +3833,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:34" ht="29.1">
+    <row r="60" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>295</v>
       </c>
@@ -3907,7 +3859,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:34" ht="72.599999999999994">
+    <row r="61" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>298</v>
       </c>
@@ -3927,7 +3879,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:34" ht="57.95">
+    <row r="62" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>302</v>
       </c>
@@ -3962,7 +3914,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:34" ht="43.5">
+    <row r="63" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>308</v>
       </c>
@@ -3985,7 +3937,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:34" ht="43.5">
+    <row r="64" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>311</v>
       </c>
@@ -4008,7 +3960,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:34" ht="57.95">
+    <row r="65" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>314</v>
       </c>
@@ -4028,7 +3980,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="1:34" ht="43.5">
+    <row r="66" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>314</v>
       </c>
@@ -4066,7 +4018,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:34" ht="43.5">
+    <row r="67" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>314</v>
       </c>
@@ -4092,7 +4044,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:34" ht="43.5">
+    <row r="68" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>324</v>
       </c>
@@ -4130,7 +4082,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="1:34" ht="43.5">
+    <row r="69" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>327</v>
       </c>
@@ -4156,7 +4108,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="70" spans="1:34" ht="101.45">
+    <row r="70" spans="1:34" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>330</v>
       </c>
@@ -4188,7 +4140,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="1:34" ht="57.95">
+    <row r="71" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>335</v>
       </c>
@@ -4211,7 +4163,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="72" spans="1:34" ht="57.95">
+    <row r="72" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>339</v>
       </c>
@@ -4231,7 +4183,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="73" spans="1:34" ht="43.5">
+    <row r="73" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>342</v>
       </c>
@@ -4251,7 +4203,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:34" ht="43.5">
+    <row r="74" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>346</v>
       </c>
@@ -4271,7 +4223,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:34" ht="72.599999999999994">
+    <row r="75" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>350</v>
       </c>
@@ -4303,7 +4255,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="1:34" ht="87">
+    <row r="76" spans="1:34" ht="87" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>355</v>
       </c>
@@ -4329,7 +4281,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="77" spans="1:34" ht="43.5">
+    <row r="77" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>358</v>
       </c>
@@ -4364,7 +4316,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="78" spans="1:34" ht="43.5">
+    <row r="78" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>362</v>
       </c>
@@ -4387,7 +4339,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:34" ht="116.1">
+    <row r="79" spans="1:34" ht="116" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>365</v>
       </c>
@@ -4425,7 +4377,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="80" spans="1:34" ht="29.1">
+    <row r="80" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>371</v>
       </c>
@@ -4451,7 +4403,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="81" spans="1:33" ht="57.95">
+    <row r="81" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>375</v>
       </c>
@@ -4474,7 +4426,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="82" spans="1:33" ht="29.1">
+    <row r="82" spans="1:33" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>378</v>
       </c>
@@ -4494,7 +4446,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:33" ht="29.1">
+    <row r="83" spans="1:33" ht="29" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>382</v>
       </c>
@@ -4529,7 +4481,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:33" ht="130.5">
+    <row r="84" spans="1:33" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>386</v>
       </c>
@@ -4552,7 +4504,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="85" spans="1:33" ht="43.5">
+    <row r="85" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>391</v>
       </c>
@@ -4578,7 +4530,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="86" spans="1:33" ht="43.5">
+    <row r="86" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>395</v>
       </c>
@@ -4598,7 +4550,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="87" spans="1:33" ht="43.5">
+    <row r="87" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>399</v>
       </c>
@@ -4618,7 +4570,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="88" spans="1:33" ht="43.5">
+    <row r="88" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>402</v>
       </c>
@@ -4641,7 +4593,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="89" spans="1:33" ht="43.5">
+    <row r="89" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>405</v>
       </c>
@@ -4661,7 +4613,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="90" spans="1:33" ht="116.1">
+    <row r="90" spans="1:33" ht="116" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>409</v>
       </c>
@@ -4681,7 +4633,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="91" spans="1:33" ht="43.5">
+    <row r="91" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>413</v>
       </c>
@@ -4701,7 +4653,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="92" spans="1:33" ht="72.599999999999994">
+    <row r="92" spans="1:33" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>417</v>
       </c>
@@ -4724,7 +4676,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="93" spans="1:33" ht="43.5">
+    <row r="93" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>421</v>
       </c>
@@ -4747,7 +4699,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="94" spans="1:33" ht="43.5">
+    <row r="94" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>426</v>
       </c>
@@ -4770,7 +4722,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="95" spans="1:33" ht="130.5">
+    <row r="95" spans="1:33" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>430</v>
       </c>
@@ -4802,7 +4754,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="96" spans="1:33" ht="43.5">
+    <row r="96" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>434</v>
       </c>
@@ -4822,7 +4774,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="97" spans="1:34" ht="43.5">
+    <row r="97" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>438</v>
       </c>
@@ -4845,7 +4797,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="98" spans="1:34" ht="43.5">
+    <row r="98" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>442</v>
       </c>
@@ -4883,318 +4835,356 @@
         <v>43</v>
       </c>
     </row>
-    <row r="99" spans="1:34" ht="43.5">
+    <row r="99" spans="1:34" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B99" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="E99" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N99" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R99" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S99" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH99" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="100" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A100" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="B99" s="9">
+      <c r="B100" s="9">
         <v>2018</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="D99" s="11" t="s">
+      <c r="D100" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E99" s="14" t="s">
+      <c r="E100" s="14" t="s">
         <v>449</v>
       </c>
-      <c r="F99" s="2" t="s">
+      <c r="F100" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G99" s="2" t="s">
+      <c r="G100" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K99" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG99" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="100" spans="1:34" ht="29.1">
-      <c r="A100" s="2" t="s">
+      <c r="K100" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG100" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="101" spans="1:34" ht="29" x14ac:dyDescent="0.35">
+      <c r="A101" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B100" s="3">
+      <c r="B101" s="3">
         <v>2018</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="D100" s="11" t="s">
+      <c r="D101" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E100" s="14" t="s">
+      <c r="E101" s="14" t="s">
         <v>452</v>
       </c>
-      <c r="K100" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O100" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="101" spans="1:34" ht="57.95">
-      <c r="A101" s="2" t="s">
+      <c r="K101" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O101" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="102" spans="1:34" ht="58" x14ac:dyDescent="0.35">
+      <c r="A102" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B102" s="2">
         <v>2017</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="D101" s="11" t="s">
+      <c r="D102" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E101" s="14" t="s">
+      <c r="E102" s="14" t="s">
         <v>455</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F102" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N101" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R101" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="102" spans="1:34" ht="87">
-      <c r="A102" s="2" t="s">
+      <c r="N102" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R102" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="103" spans="1:34" ht="87" x14ac:dyDescent="0.35">
+      <c r="A103" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="B102" s="2">
+      <c r="B103" s="2">
         <v>2020</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="D102" s="11" t="s">
+      <c r="D103" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="E102" s="14" t="s">
+      <c r="E103" s="14" t="s">
         <v>459</v>
       </c>
-      <c r="F102" s="2" t="s">
+      <c r="F103" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="H102" s="10" t="s">
+      <c r="H103" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I102" s="2" t="s">
+      <c r="I103" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="N102" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z102" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="103" spans="1:34" ht="29.1">
-      <c r="A103" s="2" t="s">
+      <c r="N103" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z103" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="104" spans="1:34" ht="29" x14ac:dyDescent="0.35">
+      <c r="A104" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="B103" s="3">
+      <c r="B104" s="3">
         <v>2020</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C104" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="D103" s="11" t="s">
+      <c r="D104" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="E103" s="14" t="s">
+      <c r="E104" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="F103" s="2" t="s">
+      <c r="F104" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K103" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="104" spans="1:34" ht="57.95">
-      <c r="A104" s="2" t="s">
+      <c r="K104" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="105" spans="1:34" ht="58" x14ac:dyDescent="0.35">
+      <c r="A105" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="B104" s="2">
+      <c r="B105" s="2">
         <v>2004</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C105" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="D104" s="11" t="s">
+      <c r="D105" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="E104" s="14" t="s">
+      <c r="E105" s="14" t="s">
         <v>466</v>
       </c>
-      <c r="H104" s="10" t="s">
+      <c r="H105" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I104" s="2" t="s">
+      <c r="I105" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="K104" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M104" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="105" spans="1:34" ht="43.5">
-      <c r="A105" s="2" t="s">
+      <c r="K105" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M105" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="106" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A106" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="B105" s="3">
-        <v>2021</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="D105" s="11" t="s">
-        <v>470</v>
-      </c>
-      <c r="E105" s="14" t="s">
-        <v>471</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J105" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE105" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="106" spans="1:34" ht="43.5">
-      <c r="A106" s="2" t="s">
-        <v>472</v>
       </c>
       <c r="B106" s="3">
         <v>2021</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D106" s="11" t="s">
         <v>470</v>
       </c>
       <c r="E106" s="14" t="s">
-        <v>474</v>
+        <v>471</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="J106" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="T106" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC106" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="107" spans="1:34" ht="57.95">
+      <c r="AE106" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="107" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="B107" s="2">
+      <c r="B107" s="3">
+        <v>2021</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="D107" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="E107" s="14" t="s">
+        <v>474</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T107" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC107" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="108" spans="1:34" ht="58" x14ac:dyDescent="0.35">
+      <c r="A108" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B108" s="2">
         <v>2017</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="D107" s="11" t="s">
+      <c r="D108" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E107" s="16" t="s">
+      <c r="E108" s="16" t="s">
         <v>476</v>
       </c>
-      <c r="N107" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O107" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH107" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="108" spans="1:34" ht="72.599999999999994">
-      <c r="A108" s="2" t="s">
+      <c r="N108" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O108" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH108" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="109" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A109" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="B108" s="2">
+      <c r="B109" s="2">
         <v>2021</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C109" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="D108" s="11" t="s">
+      <c r="D109" s="11" t="s">
         <v>479</v>
       </c>
-      <c r="E108" s="14" t="s">
+      <c r="E109" s="14" t="s">
         <v>480</v>
       </c>
-      <c r="F108" s="2" t="s">
+      <c r="F109" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G108" s="2" t="s">
+      <c r="G109" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="H108" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="I108" s="2" t="s">
+      <c r="H109" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I109" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE108" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH108" s="1" t="s">
+      <c r="J109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH109" s="1" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AH108" xr:uid="{2CFBCA1A-30D0-406A-832D-88EB6CD9ED9E}">
+  <autoFilter ref="A2:AH109" xr:uid="{2CFBCA1A-30D0-406A-832D-88EB6CD9ED9E}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AH83">
       <sortCondition ref="A3:A83"/>
       <sortCondition descending="1" ref="B3:B83"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AH108">
-    <sortCondition ref="A3:A108"/>
-    <sortCondition descending="1" ref="B3:B108"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AH109">
+    <sortCondition ref="A3:A109"/>
+    <sortCondition descending="1" ref="B3:B109"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="J1:N1"/>
@@ -5202,70 +5192,37 @@
     <mergeCell ref="AC1:AH1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H106 H109:H1048576 H56:H104 H1:H54">
-    <cfRule type="containsText" dxfId="17" priority="27" operator="containsText" text="tbc">
+  <conditionalFormatting sqref="H1:H54">
+    <cfRule type="containsText" dxfId="8" priority="27" operator="containsText" text="tbc">
       <formula>NOT(ISERROR(SEARCH("tbc",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="42" operator="containsText" text="to see">
+    <cfRule type="containsText" dxfId="7" priority="42" operator="containsText" text="to see">
       <formula>NOT(ISERROR(SEARCH("to see",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="43" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="6" priority="43" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="44" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="5" priority="44" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI3:AI89">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="pb">
-      <formula>NOT(ISERROR(SEARCH("pb",AI3)))</formula>
+  <conditionalFormatting sqref="H56:H1048576">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="tbc">
+      <formula>NOT(ISERROR(SEARCH("tbc",H56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="to see">
+      <formula>NOT(ISERROR(SEARCH("to see",H56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",H56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",H56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI90:AI99">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="pb">
-      <formula>NOT(ISERROR(SEARCH("pb",AI90)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H105">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="tbc">
-      <formula>NOT(ISERROR(SEARCH("tbc",H105)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="to see">
-      <formula>NOT(ISERROR(SEARCH("to see",H105)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",H105)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",H105)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H107">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="tbc">
-      <formula>NOT(ISERROR(SEARCH("tbc",H107)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="to see">
-      <formula>NOT(ISERROR(SEARCH("to see",H107)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",H107)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",H107)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H108">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="tbc">
-      <formula>NOT(ISERROR(SEARCH("tbc",H108)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="to see">
-      <formula>NOT(ISERROR(SEARCH("to see",H108)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",H108)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",H108)))</formula>
+  <conditionalFormatting sqref="AI3:AI100">
+    <cfRule type="containsText" dxfId="0" priority="13" operator="containsText" text="pb">
+      <formula>NOT(ISERROR(SEARCH("pb",AI3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -5278,14 +5235,14 @@
     <hyperlink ref="E62" r:id="rId7" xr:uid="{027C1889-F71D-41F9-AAB3-710415514B9A}"/>
     <hyperlink ref="E64" r:id="rId8" xr:uid="{7F16FD1B-410C-4736-B12B-538ED1B1CA4A}"/>
     <hyperlink ref="E73" r:id="rId9" xr:uid="{96547B7D-03C7-4FB0-871E-52924B32F313}"/>
-    <hyperlink ref="E100" r:id="rId10" xr:uid="{669A4DC3-F305-4158-821E-9DDF7FA031D9}"/>
+    <hyperlink ref="E101" r:id="rId10" xr:uid="{669A4DC3-F305-4158-821E-9DDF7FA031D9}"/>
     <hyperlink ref="E74" r:id="rId11" xr:uid="{494A117E-C8A0-4172-AB2B-CBDB4AD3EB9C}"/>
     <hyperlink ref="E63" r:id="rId12" xr:uid="{099984D8-6082-40F0-9E84-E49E1BB5574C}"/>
     <hyperlink ref="E43" r:id="rId13" xr:uid="{BE14CD70-8EAE-48EB-8DBB-26D14DD3169E}"/>
     <hyperlink ref="E91" r:id="rId14" xr:uid="{E6E9C87F-4F38-4FB1-B153-C74AAFDF2F2B}"/>
     <hyperlink ref="E85" r:id="rId15" xr:uid="{E400C837-FFD8-481F-B368-EE894FCDA1BC}"/>
     <hyperlink ref="E87" r:id="rId16" xr:uid="{2DA9E77C-A279-407D-A22A-DBB8036D095C}"/>
-    <hyperlink ref="E103" r:id="rId17" xr:uid="{4B54B9BB-8F33-47B5-A90B-B10DB08E0813}"/>
+    <hyperlink ref="E104" r:id="rId17" xr:uid="{4B54B9BB-8F33-47B5-A90B-B10DB08E0813}"/>
     <hyperlink ref="E7" r:id="rId18" xr:uid="{95E7CD7F-AF88-45EC-8F37-E5E9D1EF1034}"/>
     <hyperlink ref="E17" r:id="rId19" xr:uid="{E0EBEC91-B437-46E7-825D-8215BE6C2171}"/>
     <hyperlink ref="E31" r:id="rId20" xr:uid="{112A3FCC-C815-4772-8173-B88F7D873D08}"/>
@@ -5312,7 +5269,7 @@
     <hyperlink ref="E21" r:id="rId41" xr:uid="{C0C54509-B25E-4A61-A33B-9BC669C139B1}"/>
     <hyperlink ref="E24" r:id="rId42" xr:uid="{17CBDD15-89FB-4714-8293-10AA629C94AE}"/>
     <hyperlink ref="E25" r:id="rId43" xr:uid="{56704F90-1A3C-477A-B777-D214530F6C5F}"/>
-    <hyperlink ref="E108" r:id="rId44" xr:uid="{911F88E0-33FE-4735-A223-7A0A51988D6C}"/>
+    <hyperlink ref="E109" r:id="rId44" xr:uid="{911F88E0-33FE-4735-A223-7A0A51988D6C}"/>
     <hyperlink ref="E30" r:id="rId45" location=":~:text=Both%20scenarios%20show%20that%2C%20at,)%2C%20while%20nuclear%20power%20decreases." xr:uid="{EA05B2F9-69A3-4830-B3AD-7E1B7CE631D1}"/>
     <hyperlink ref="E35" r:id="rId46" xr:uid="{25B0BDC6-0A3E-48D3-A3E8-32E6F3075DCC}"/>
     <hyperlink ref="E36" r:id="rId47" xr:uid="{67A7E60B-B849-4080-A8A3-0BBA26FED531}"/>
@@ -5344,11 +5301,11 @@
     <hyperlink ref="E95" r:id="rId73" location=":~:text=Windstorms%20are%20amongst%20the%20most,annual%20losses%20in%20the%20EU.&amp;text=As%20a%20consequence%2C%20it%20is,rise%20due%20to%20climate%20change." xr:uid="{84766123-8B9C-40D7-9092-EE32EC59F2D3}"/>
     <hyperlink ref="E97" r:id="rId74" xr:uid="{EE1C6824-4127-49BF-856B-54D15A26EEC3}"/>
     <hyperlink ref="E27" r:id="rId75" xr:uid="{8772BA96-ED44-4481-A6D6-CAB4C1D2D36D}"/>
-    <hyperlink ref="E99" r:id="rId76" xr:uid="{A8B1A50A-41B3-4028-8B6D-55BA1E74EF06}"/>
+    <hyperlink ref="E100" r:id="rId76" xr:uid="{A8B1A50A-41B3-4028-8B6D-55BA1E74EF06}"/>
     <hyperlink ref="E70" r:id="rId77" xr:uid="{7A6C35C0-065D-48C9-81B5-5BAC2E227370}"/>
-    <hyperlink ref="E105" r:id="rId78" xr:uid="{18FEDC5F-D897-4BD3-B5F5-B23D6192D5C7}"/>
-    <hyperlink ref="E106" r:id="rId79" xr:uid="{188633F7-D468-4FF1-B629-6E1DEC4631EE}"/>
-    <hyperlink ref="E107" r:id="rId80" xr:uid="{6FAF70A0-3FCF-454F-9682-BAB8A8C9D3E7}"/>
+    <hyperlink ref="E106" r:id="rId78" xr:uid="{18FEDC5F-D897-4BD3-B5F5-B23D6192D5C7}"/>
+    <hyperlink ref="E107" r:id="rId79" xr:uid="{188633F7-D468-4FF1-B629-6E1DEC4631EE}"/>
+    <hyperlink ref="E108" r:id="rId80" xr:uid="{6FAF70A0-3FCF-454F-9682-BAB8A8C9D3E7}"/>
     <hyperlink ref="E79" r:id="rId81" xr:uid="{D9A56F1D-2229-42A5-84AC-9DA4A78FF246}"/>
     <hyperlink ref="E42" r:id="rId82" xr:uid="{44C7D96C-57CD-4E32-B593-A7F8B9769E84}"/>
     <hyperlink ref="E54" r:id="rId83" xr:uid="{961F3F75-E073-4BB0-A98B-0BE784E6D0A8}"/>
@@ -5359,24 +5316,25 @@
     <hyperlink ref="E50" r:id="rId88" xr:uid="{88DFAFA3-C726-468A-934C-491527C128D6}"/>
     <hyperlink ref="E48" r:id="rId89" xr:uid="{F591CC07-7435-4E15-9D93-39528ACCE89B}"/>
     <hyperlink ref="E75" r:id="rId90" xr:uid="{ED87634C-0B58-4EAF-BEDB-2A48A969155C}"/>
-    <hyperlink ref="E104" r:id="rId91" xr:uid="{C77ED42E-2BAE-4561-B014-7D5CCCD7300B}"/>
+    <hyperlink ref="E105" r:id="rId91" xr:uid="{C77ED42E-2BAE-4561-B014-7D5CCCD7300B}"/>
     <hyperlink ref="E52" r:id="rId92" xr:uid="{AE60E41F-78E6-4C0B-99CC-9B9F011A14D2}"/>
     <hyperlink ref="E22" r:id="rId93" xr:uid="{D2CDFB65-960D-4324-9309-D75DB0AE6DE1}"/>
     <hyperlink ref="E32" r:id="rId94" xr:uid="{78010408-7D00-4480-9D3C-B780BB49E81D}"/>
     <hyperlink ref="E8" r:id="rId95" xr:uid="{2220BCD0-A5B0-4A1D-AA6D-A1D41EBDE3CE}"/>
-    <hyperlink ref="E101" r:id="rId96" xr:uid="{3338E87A-5ECB-4F9B-ACE2-2EC0716ABFED}"/>
+    <hyperlink ref="E102" r:id="rId96" xr:uid="{3338E87A-5ECB-4F9B-ACE2-2EC0716ABFED}"/>
     <hyperlink ref="E80" r:id="rId97" xr:uid="{C18AFA26-2EB1-499D-B2B4-72BB9C037E10}"/>
     <hyperlink ref="E26" r:id="rId98" xr:uid="{7D25A591-E8A8-418A-A32D-CDEB86ABCE99}"/>
     <hyperlink ref="E28" r:id="rId99" xr:uid="{2582EDBD-D337-4487-BD2B-35A6BA106688}"/>
     <hyperlink ref="E76" r:id="rId100" xr:uid="{93645E69-F230-4737-B909-AF6297441E90}"/>
     <hyperlink ref="E57" r:id="rId101" xr:uid="{A4270E10-FA55-4CD6-89BD-993EB73F11ED}"/>
     <hyperlink ref="E33" r:id="rId102" xr:uid="{7C482A88-1330-4A10-AE85-2F21D5F0D01B}"/>
-    <hyperlink ref="E102" r:id="rId103" xr:uid="{82E79761-A535-494D-98AA-10AEED4B01D5}"/>
+    <hyperlink ref="E103" r:id="rId103" xr:uid="{82E79761-A535-494D-98AA-10AEED4B01D5}"/>
     <hyperlink ref="E58" r:id="rId104" xr:uid="{74A01E59-FEDC-471C-A936-DCE757B765DE}"/>
     <hyperlink ref="E77" r:id="rId105" xr:uid="{C16C0228-218F-4349-9E17-C55FCC0E4848}"/>
     <hyperlink ref="E83" r:id="rId106" xr:uid="{16CF4C79-2C66-473B-8376-0E52D53979DE}"/>
+    <hyperlink ref="E99" r:id="rId107" xr:uid="{6B3A7836-3287-4B71-BAE9-EBE88E438E91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId107"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId108"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add an entry to the litterature review spreadsheet (#247)
* Add an entry to the litterature review spreadsheet

Add to the spreadsheet the following reference: Luo, T., Cheng, Y., Falzon, J. et al. A framework to assess multi-hazard physical climate risk for power generation projects from publicly-accessible sources. Commun Earth Environ 4, 117 (2023). https://doi.org/10.1038/s43247-023-00782-w

Signed-off-by: EglantineGiraud <eglantine.giraud@gmail.com>

* Add an entry to the litterature review spreadsheet

Add to the spreadsheet the following reference: Luo, T., Cheng, Y., Falzon, J. et al. A framework to assess multi-hazard physical climate risk for power generation projects from publicly-accessible sources. Commun Earth Environ 4, 117 (2023). https://doi.org/10.1038/s43247-023-00782-w

Signed-off-by: EglantineGiraud <eglantine.giraud@gmail.com>

---------

Signed-off-by: EglantineGiraud <eglantine.giraud@gmail.com>
</commit_message>
<xml_diff>
--- a/methodology/literature/Literature_review.xlsx
+++ b/methodology/literature/Literature_review.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eglan\OneDrive\Documents\GitHub\physrisk\methodology\literature\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2aaf0d77d3bf0a19/Documents/GitHub/physrisk/methodology/literature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0706C6C0-083C-45A5-8CF9-7C492524EE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{0706C6C0-083C-45A5-8CF9-7C492524EE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1922ECF-3209-4E36-B091-5BCDB53FACA2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5E70EA40-22C4-4E82-B7B8-60E8844517C7}"/>
   </bookViews>
@@ -1499,7 +1499,7 @@
     <t>Communications Earth &amp; Environment</t>
   </si>
   <si>
-    <t xml:space="preserve">This article introduces a scalable and transparent methodology that enables multi-hazard physical climate risk assessments for any thermal or hydro power generation project. The methodology relies on basic power plant type and geolocation data inputs, publicly-available climate datasets, and hazard- and technology-specific vulnerability factors, to translate hazard severity into generation losses. </t>
+    <t>Scalable and transparent methodology that enables multi-hazard physical climate risk assessments for any thermal or hydro power generation project. It relies on basic power plant type and geolocation data inputs, publicly-available climate datasets, and hazard- and technology-specific vulnerability factors, to translate hazard severity into generation losses.</t>
   </si>
 </sst>
 </file>
@@ -1674,39 +1674,11 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2054,7 +2026,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3859,128 +3831,146 @@
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:34" ht="87" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B61" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH61" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B62" s="3">
         <v>2009</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="D62" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E62" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="K61" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="62" spans="1:34" ht="58" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
+      <c r="K62" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:34" ht="58" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="B62" s="3">
-        <v>2020</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="H62" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="K62" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z62" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG62" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="63" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
-        <v>308</v>
       </c>
       <c r="B63" s="3">
         <v>2020</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E63" s="14" t="s">
-        <v>310</v>
+        <v>304</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>307</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>43</v>
       </c>
       <c r="Z63" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG63" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B64" s="3">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D64" s="11" t="s">
         <v>132</v>
       </c>
       <c r="E64" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z64" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B65" s="3">
+        <v>2019</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E65" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="K64" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z64" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="65" spans="1:34" ht="58" x14ac:dyDescent="0.35">
-      <c r="A65" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="B65" s="3">
-        <v>2010</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>317</v>
-      </c>
       <c r="K65" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="66" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="Z65" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>314</v>
       </c>
@@ -3988,33 +3978,15 @@
         <v>2010</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="H66" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="I66" s="2" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O66" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z66" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG66" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4023,548 +3995,566 @@
         <v>314</v>
       </c>
       <c r="B67" s="3">
-        <v>2004</v>
+        <v>2010</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>319</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>323</v>
+        <v>320</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="H67" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>307</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="O67" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="Z67" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AE67" s="1" t="s">
+      <c r="AG67" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="B68" s="2">
-        <v>2015</v>
+        <v>314</v>
+      </c>
+      <c r="B68" s="3">
+        <v>2004</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>52</v>
+        <v>319</v>
       </c>
       <c r="E68" s="14" t="s">
-        <v>326</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="H68" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="J68" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T68" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD68" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z68" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE68" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="B69" s="3">
-        <v>2011</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
+      </c>
+      <c r="B69" s="2">
+        <v>2015</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>329</v>
+        <v>326</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="H69" s="10" t="s">
         <v>48</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="L69" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="70" spans="1:34" ht="101.5" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T69" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD69" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B70" s="3">
-        <v>2020</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>331</v>
+        <v>2011</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>328</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>332</v>
+        <v>61</v>
       </c>
       <c r="E70" s="14" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="H70" s="10" t="s">
         <v>48</v>
       </c>
       <c r="I70" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="71" spans="1:34" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B71" s="3">
+        <v>2020</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I71" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="K70" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L70" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P70" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="71" spans="1:34" ht="58" x14ac:dyDescent="0.35">
-      <c r="A71" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="B71" s="3">
-        <v>2010</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D71" s="11" t="s">
-        <v>337</v>
-      </c>
-      <c r="E71" s="14" t="s">
-        <v>338</v>
-      </c>
       <c r="K71" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AG71" s="1" t="s">
+      <c r="L71" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P71" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B72" s="3">
+        <v>2010</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG72" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" spans="1:34" ht="58" x14ac:dyDescent="0.35">
+      <c r="A73" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B73" s="2">
         <v>2014</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="D72" s="11" t="s">
+      <c r="D73" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E72" s="14" t="s">
+      <c r="E73" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="O72" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="73" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="B73" s="3">
-        <v>2014</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="E73" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="K73" s="1" t="s">
+      <c r="O73" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B74" s="3">
         <v>2014</v>
       </c>
       <c r="C74" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="75" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B75" s="3">
+        <v>2014</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="D74" s="11" t="s">
+      <c r="D75" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="E74" s="14" t="s">
+      <c r="E75" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="K74" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="75" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="2" t="s">
+      <c r="K75" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B76" s="2">
         <v>2014</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D75" s="11" t="s">
+      <c r="D76" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="E75" s="14" t="s">
+      <c r="E76" s="14" t="s">
         <v>353</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="H75" s="10" t="s">
+      <c r="H76" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I75" s="2" t="s">
+      <c r="I76" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="K75" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q75" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="76" spans="1:34" ht="87" x14ac:dyDescent="0.35">
-      <c r="A76" s="2" t="s">
+      <c r="K76" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q76" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="77" spans="1:34" ht="87" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B77" s="2">
         <v>2020</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="D76" s="11" t="s">
+      <c r="D77" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E76" s="14" t="s">
+      <c r="E77" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="J76" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T76" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC76" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="77" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B77" s="2">
-        <v>2018</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E77" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="H77" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="N77" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R77" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z77" s="1" t="s">
+      <c r="J77" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T77" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC77" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="78" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B78" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="H78" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="N78" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R78" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z78" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B79" s="2">
         <v>2013</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="D78" s="11" t="s">
+      <c r="D79" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="E78" s="14" t="s">
+      <c r="E79" s="14" t="s">
         <v>364</v>
       </c>
-      <c r="O78" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH78" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="79" spans="1:34" ht="116" x14ac:dyDescent="0.35">
-      <c r="A79" s="2" t="s">
+      <c r="O79" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH79" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="80" spans="1:34" ht="116" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B80" s="2">
         <v>2022</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="D79" s="11" t="s">
+      <c r="D80" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="E79" s="14" t="s">
+      <c r="E80" s="14" t="s">
         <v>368</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="G80" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="H79" s="10" t="s">
+      <c r="H80" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="I80" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="J79" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T79" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD79" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="80" spans="1:34" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="2" t="s">
+      <c r="J80" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T80" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD80" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="81" spans="1:33" ht="29" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B81" s="2">
         <v>2021</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="D80" s="11" t="s">
+      <c r="D81" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="E80" s="14" t="s">
+      <c r="E81" s="14" t="s">
         <v>373</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F81" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="J80" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R80" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="81" spans="1:33" ht="58" x14ac:dyDescent="0.35">
-      <c r="A81" s="2" t="s">
+      <c r="J81" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R81" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="82" spans="1:33" ht="58" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B82" s="3">
         <v>2011</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="D81" s="11" t="s">
+      <c r="D82" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="E81" s="14" t="s">
+      <c r="E82" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F82" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="P81" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="82" spans="1:33" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B82" s="3">
-        <v>2020</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>380</v>
-      </c>
-      <c r="E82" s="14" t="s">
-        <v>381</v>
-      </c>
-      <c r="R82" s="1" t="s">
+      <c r="P82" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="83" spans="1:33" ht="29" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B83" s="3">
+        <v>2020</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="R83" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="84" spans="1:33" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B84" s="2">
         <v>2015</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="D83" s="11" t="s">
+      <c r="D84" s="11" t="s">
         <v>384</v>
       </c>
-      <c r="E83" s="14" t="s">
+      <c r="E84" s="14" t="s">
         <v>385</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H83" s="10" t="s">
+      <c r="H84" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I83" s="2" t="s">
+      <c r="I84" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="N83" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R83" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z83" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="84" spans="1:33" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="3" t="s">
+      <c r="N84" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R84" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z84" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="85" spans="1:33" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A85" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="B84" s="3">
+      <c r="B85" s="3">
         <v>2018</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="D84" s="11" t="s">
+      <c r="D85" s="11" t="s">
         <v>388</v>
       </c>
-      <c r="E84" s="14" t="s">
+      <c r="E85" s="14" t="s">
         <v>389</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="I85" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="K84" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="85" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A85" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="B85" s="3">
-        <v>2014</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>393</v>
-      </c>
-      <c r="E85" s="14" t="s">
-        <v>394</v>
-      </c>
       <c r="K85" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z85" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG85" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="86" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B86" s="9">
-        <v>2016</v>
+        <v>391</v>
+      </c>
+      <c r="B86" s="3">
+        <v>2014</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="D86" s="12" t="s">
-        <v>397</v>
+        <v>392</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>393</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="K86" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z86" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG86" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="87" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="B87" s="3">
-        <v>2019</v>
+        <v>395</v>
+      </c>
+      <c r="B87" s="9">
+        <v>2016</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D87" s="11" t="s">
-        <v>132</v>
+        <v>396</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>397</v>
       </c>
       <c r="E87" s="14" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="K87" s="1" t="s">
         <v>43</v>
@@ -4572,304 +4562,286 @@
     </row>
     <row r="88" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B88" s="3">
         <v>2019</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>402</v>
+        <v>132</v>
       </c>
       <c r="E88" s="14" t="s">
-        <v>404</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB88" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="K88" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="89" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B89" s="3">
+        <v>2019</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB89" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="90" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A90" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B90" s="2">
         <v>2017</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="D89" s="11" t="s">
+      <c r="D90" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="E89" s="14" t="s">
+      <c r="E90" s="14" t="s">
         <v>408</v>
       </c>
-      <c r="O89" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="90" spans="1:33" ht="116" x14ac:dyDescent="0.35">
-      <c r="A90" s="2" t="s">
+      <c r="O90" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="91" spans="1:33" ht="116" x14ac:dyDescent="0.35">
+      <c r="A91" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B90" s="3">
+      <c r="B91" s="3">
         <v>2020</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="D90" s="11" t="s">
+      <c r="D91" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="E90" s="14" t="s">
+      <c r="E91" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="P90" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="91" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A91" s="2" t="s">
+      <c r="P91" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="92" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A92" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="B91" s="3">
+      <c r="B92" s="3">
         <v>2018</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="D91" s="11" t="s">
+      <c r="D92" s="11" t="s">
         <v>415</v>
       </c>
-      <c r="E91" s="14" t="s">
+      <c r="E92" s="14" t="s">
         <v>416</v>
       </c>
-      <c r="K91" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="92" spans="1:33" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A92" s="2" t="s">
+      <c r="K92" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="93" spans="1:33" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A93" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B92" s="3">
+      <c r="B93" s="3">
         <v>2008</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D92" s="11" t="s">
+      <c r="D93" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="E92" s="14" t="s">
+      <c r="E93" s="14" t="s">
         <v>420</v>
       </c>
-      <c r="K92" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG92" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="93" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A93" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="B93" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="D93" s="11" t="s">
-        <v>423</v>
-      </c>
-      <c r="E93" s="14" t="s">
-        <v>424</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="P93" s="1" t="s">
+      <c r="K93" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG93" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="94" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B94" s="3">
+        <v>2019</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>423</v>
+      </c>
+      <c r="E94" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="P94" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="95" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A95" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B95" s="3">
         <v>2013</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="D94" s="11" t="s">
+      <c r="D95" s="11" t="s">
         <v>428</v>
       </c>
-      <c r="E94" s="14" t="s">
+      <c r="E95" s="14" t="s">
         <v>429</v>
       </c>
-      <c r="K94" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P94" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="95" spans="1:33" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A95" s="2" t="s">
+      <c r="K95" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P95" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="96" spans="1:33" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A96" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B96" s="3">
         <v>2019</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="D95" s="11" t="s">
+      <c r="D96" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E95" s="14" t="s">
+      <c r="E96" s="14" t="s">
         <v>432</v>
       </c>
-      <c r="F95" s="2" t="s">
+      <c r="F96" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G95" s="2" t="s">
+      <c r="G96" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="M95" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T95" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD95" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="96" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A96" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B96" s="3">
-        <v>2018</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="D96" s="11" t="s">
-        <v>436</v>
-      </c>
-      <c r="E96" s="14" t="s">
-        <v>437</v>
-      </c>
-      <c r="AC96" s="1" t="s">
+      <c r="M96" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T96" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD96" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="97" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B97" s="3">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="E97" s="14" t="s">
-        <v>441</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="P97" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="AC97" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="98" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B98" s="3">
+        <v>2020</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D98" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="E98" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="P98" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="99" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A99" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B99" s="3">
         <v>2017</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="D98" s="11" t="s">
+      <c r="D99" s="11" t="s">
         <v>444</v>
       </c>
-      <c r="E98" s="14" t="s">
+      <c r="E99" s="14" t="s">
         <v>445</v>
       </c>
-      <c r="F98" s="2" t="s">
+      <c r="F99" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="G99" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="H98" s="10" t="s">
+      <c r="H99" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="K98" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T98" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V98" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD98" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="99" spans="1:34" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A99" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="B99" s="3">
-        <v>2023</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="D99" s="11" t="s">
-        <v>485</v>
-      </c>
-      <c r="E99" s="14" t="s">
-        <v>484</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>486</v>
-      </c>
       <c r="K99" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L99" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N99" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R99" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S99" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH99" s="1" t="s">
+      <c r="T99" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V99" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD99" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5177,9 +5149,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:AH109" xr:uid="{2CFBCA1A-30D0-406A-832D-88EB6CD9ED9E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AH83">
-      <sortCondition ref="A3:A83"/>
-      <sortCondition descending="1" ref="B3:B83"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AH84">
+      <sortCondition ref="A3:A84"/>
+      <sortCondition descending="1" ref="B3:B84"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AH109">
@@ -5192,32 +5164,18 @@
     <mergeCell ref="AC1:AH1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H1:H54">
-    <cfRule type="containsText" dxfId="8" priority="27" operator="containsText" text="tbc">
+  <conditionalFormatting sqref="H1:H54 H56:H1048576">
+    <cfRule type="containsText" dxfId="4" priority="27" operator="containsText" text="tbc">
       <formula>NOT(ISERROR(SEARCH("tbc",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="42" operator="containsText" text="to see">
+    <cfRule type="containsText" dxfId="3" priority="42" operator="containsText" text="to see">
       <formula>NOT(ISERROR(SEARCH("to see",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="43" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="2" priority="43" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="44" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="1" priority="44" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",H1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H56:H1048576">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="tbc">
-      <formula>NOT(ISERROR(SEARCH("tbc",H56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="to see">
-      <formula>NOT(ISERROR(SEARCH("to see",H56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",H56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",H56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3:AI100">
@@ -5228,26 +5186,26 @@
   <hyperlinks>
     <hyperlink ref="E44" r:id="rId1" xr:uid="{BD65012E-0145-4F39-AF56-E26BDA497D98}"/>
     <hyperlink ref="E49" r:id="rId2" xr:uid="{AF4909F5-020E-429B-AD47-0D2FA183A729}"/>
-    <hyperlink ref="E98" r:id="rId3" xr:uid="{49DB0C1A-3930-4215-BD94-23086F897C5B}"/>
+    <hyperlink ref="E99" r:id="rId3" xr:uid="{49DB0C1A-3930-4215-BD94-23086F897C5B}"/>
     <hyperlink ref="E14" r:id="rId4" xr:uid="{ACE54CBE-A8CD-4089-9537-B2B3C2A30C02}"/>
     <hyperlink ref="E34" r:id="rId5" xr:uid="{4B5CFAED-68B4-49DE-B7BF-1F7117BD90B1}"/>
     <hyperlink ref="E6" r:id="rId6" xr:uid="{E2EDA215-C448-4F2C-9BDF-E6AC9544297A}"/>
-    <hyperlink ref="E62" r:id="rId7" xr:uid="{027C1889-F71D-41F9-AAB3-710415514B9A}"/>
-    <hyperlink ref="E64" r:id="rId8" xr:uid="{7F16FD1B-410C-4736-B12B-538ED1B1CA4A}"/>
-    <hyperlink ref="E73" r:id="rId9" xr:uid="{96547B7D-03C7-4FB0-871E-52924B32F313}"/>
+    <hyperlink ref="E63" r:id="rId7" xr:uid="{027C1889-F71D-41F9-AAB3-710415514B9A}"/>
+    <hyperlink ref="E65" r:id="rId8" xr:uid="{7F16FD1B-410C-4736-B12B-538ED1B1CA4A}"/>
+    <hyperlink ref="E74" r:id="rId9" xr:uid="{96547B7D-03C7-4FB0-871E-52924B32F313}"/>
     <hyperlink ref="E101" r:id="rId10" xr:uid="{669A4DC3-F305-4158-821E-9DDF7FA031D9}"/>
-    <hyperlink ref="E74" r:id="rId11" xr:uid="{494A117E-C8A0-4172-AB2B-CBDB4AD3EB9C}"/>
-    <hyperlink ref="E63" r:id="rId12" xr:uid="{099984D8-6082-40F0-9E84-E49E1BB5574C}"/>
+    <hyperlink ref="E75" r:id="rId11" xr:uid="{494A117E-C8A0-4172-AB2B-CBDB4AD3EB9C}"/>
+    <hyperlink ref="E64" r:id="rId12" xr:uid="{099984D8-6082-40F0-9E84-E49E1BB5574C}"/>
     <hyperlink ref="E43" r:id="rId13" xr:uid="{BE14CD70-8EAE-48EB-8DBB-26D14DD3169E}"/>
-    <hyperlink ref="E91" r:id="rId14" xr:uid="{E6E9C87F-4F38-4FB1-B153-C74AAFDF2F2B}"/>
-    <hyperlink ref="E85" r:id="rId15" xr:uid="{E400C837-FFD8-481F-B368-EE894FCDA1BC}"/>
-    <hyperlink ref="E87" r:id="rId16" xr:uid="{2DA9E77C-A279-407D-A22A-DBB8036D095C}"/>
+    <hyperlink ref="E92" r:id="rId14" xr:uid="{E6E9C87F-4F38-4FB1-B153-C74AAFDF2F2B}"/>
+    <hyperlink ref="E86" r:id="rId15" xr:uid="{E400C837-FFD8-481F-B368-EE894FCDA1BC}"/>
+    <hyperlink ref="E88" r:id="rId16" xr:uid="{2DA9E77C-A279-407D-A22A-DBB8036D095C}"/>
     <hyperlink ref="E104" r:id="rId17" xr:uid="{4B54B9BB-8F33-47B5-A90B-B10DB08E0813}"/>
     <hyperlink ref="E7" r:id="rId18" xr:uid="{95E7CD7F-AF88-45EC-8F37-E5E9D1EF1034}"/>
     <hyperlink ref="E17" r:id="rId19" xr:uid="{E0EBEC91-B437-46E7-825D-8215BE6C2171}"/>
     <hyperlink ref="E31" r:id="rId20" xr:uid="{112A3FCC-C815-4772-8173-B88F7D873D08}"/>
     <hyperlink ref="E9" r:id="rId21" xr:uid="{4854D465-9E0A-4347-AD98-8E15B7E5738A}"/>
-    <hyperlink ref="E84" r:id="rId22" xr:uid="{64C0BA33-5499-4C63-B12E-81F12B31EDA7}"/>
+    <hyperlink ref="E85" r:id="rId22" xr:uid="{64C0BA33-5499-4C63-B12E-81F12B31EDA7}"/>
     <hyperlink ref="E55" r:id="rId23" xr:uid="{24D838B3-143A-420F-957C-DE13E6EC7DA7}"/>
     <hyperlink ref="E23" r:id="rId24" xr:uid="{84C2724B-0FD0-44F6-930F-74941327DE29}"/>
     <hyperlink ref="E60" r:id="rId25" xr:uid="{3587DC42-4120-4C66-82F1-9DDA6C10995A}"/>
@@ -5255,7 +5213,7 @@
     <hyperlink ref="E5" r:id="rId27" xr:uid="{D155804D-0F52-4AA4-8C6A-118FF2215B36}"/>
     <hyperlink ref="E18" r:id="rId28" xr:uid="{FFC3EF4B-5030-409E-B750-5077897D1049}"/>
     <hyperlink ref="E45" r:id="rId29" xr:uid="{E21268E4-AA81-4C81-885D-427B28ABA286}"/>
-    <hyperlink ref="E92" r:id="rId30" xr:uid="{3890E093-D0A4-4ED4-BA06-8B46D2FB51EA}"/>
+    <hyperlink ref="E93" r:id="rId30" xr:uid="{3890E093-D0A4-4ED4-BA06-8B46D2FB51EA}"/>
     <hyperlink ref="E4" r:id="rId31" xr:uid="{F8A2D380-5289-43B2-BC8E-58CF7CF41316}"/>
     <hyperlink ref="E3" r:id="rId32" xr:uid="{AF91C158-6F0D-4129-9159-F2DAC33C699C}"/>
     <hyperlink ref="E10" r:id="rId33" location=":~:text=In%20general%2C%20the%20climate%20projections,%2C%20Malta%2C%20Italy%20and%20Turkey." xr:uid="{21238528-DB3C-40B7-89E7-E94F3F7825E0}"/>
@@ -5276,63 +5234,63 @@
     <hyperlink ref="E37" r:id="rId48" xr:uid="{AA84D5F7-75D4-4C61-BFDC-14C80366D23F}"/>
     <hyperlink ref="E38" r:id="rId49" xr:uid="{9161355B-B241-459F-BA2B-043C2652F90E}"/>
     <hyperlink ref="E39" r:id="rId50" xr:uid="{8D02E594-58BD-4D44-A4F4-D0C776727581}"/>
-    <hyperlink ref="E90" r:id="rId51" xr:uid="{DE5010F2-3196-4D97-881F-4E21C532D746}"/>
+    <hyperlink ref="E91" r:id="rId51" xr:uid="{DE5010F2-3196-4D97-881F-4E21C532D746}"/>
     <hyperlink ref="E41" r:id="rId52" xr:uid="{112B2935-AA4C-4B24-AD5C-E960962C6888}"/>
     <hyperlink ref="E46" r:id="rId53" xr:uid="{75B4D416-B55F-4D29-BB1F-E5FE365C412C}"/>
     <hyperlink ref="E51" r:id="rId54" xr:uid="{C3C3A709-15B9-4C33-A76D-ECC5637087DA}"/>
     <hyperlink ref="E53" r:id="rId55" xr:uid="{8E8B55AA-3EE4-4E34-AB2D-CDC8148E3CEA}"/>
     <hyperlink ref="E59" r:id="rId56" xr:uid="{A4BD1F52-6647-4216-8B26-7A4EE1854871}"/>
-    <hyperlink ref="E61" r:id="rId57" xr:uid="{40A90B0A-E641-4392-BFB4-5E7D7F55C016}"/>
-    <hyperlink ref="E65" r:id="rId58" xr:uid="{41CA1564-7354-45C8-A034-1B2EA1C8BBB0}"/>
+    <hyperlink ref="E62" r:id="rId57" xr:uid="{40A90B0A-E641-4392-BFB4-5E7D7F55C016}"/>
+    <hyperlink ref="E66" r:id="rId58" xr:uid="{41CA1564-7354-45C8-A034-1B2EA1C8BBB0}"/>
     <hyperlink ref="E56" r:id="rId59" xr:uid="{A8312434-A525-446F-8B2D-252B9169DE2A}"/>
-    <hyperlink ref="E67" r:id="rId60" xr:uid="{EE454482-8FED-4527-B986-77CD9C1F36C3}"/>
-    <hyperlink ref="E69" r:id="rId61" xr:uid="{4674AB5A-30F3-45D8-A76E-5D2DA2947D26}"/>
-    <hyperlink ref="E71" r:id="rId62" xr:uid="{6D1483F5-F282-415F-9759-DD789E670422}"/>
-    <hyperlink ref="E72" r:id="rId63" xr:uid="{7D4750D7-9B5F-418F-A8E0-1130FCCD84BF}"/>
-    <hyperlink ref="E78" r:id="rId64" xr:uid="{4DB7F4FC-198A-4F7C-99B5-E7956C26D0B4}"/>
-    <hyperlink ref="E81" r:id="rId65" xr:uid="{57799A75-4C8E-4C23-89A7-56A5834C31EE}"/>
-    <hyperlink ref="E82" r:id="rId66" xr:uid="{56C7BD61-7179-492F-B56F-8CB6DDCEF01A}"/>
-    <hyperlink ref="E86" r:id="rId67" xr:uid="{A62E077C-F1ED-4CCF-9B4D-44094647CCEB}"/>
-    <hyperlink ref="E88" r:id="rId68" xr:uid="{657B8500-1668-4027-AD3E-41D375A29A2F}"/>
-    <hyperlink ref="E89" r:id="rId69" xr:uid="{A51EE9E5-D6F9-4402-88D6-6938FEAAF425}"/>
-    <hyperlink ref="E93" r:id="rId70" xr:uid="{DAADEE44-3705-4408-AE31-5114CF9789AE}"/>
-    <hyperlink ref="E94" r:id="rId71" xr:uid="{2652C579-F57A-4A18-99E0-0CCE2D98D1BE}"/>
-    <hyperlink ref="E96" r:id="rId72" xr:uid="{F6E106D7-51E3-4796-8BCC-F62B4665CA66}"/>
-    <hyperlink ref="E95" r:id="rId73" location=":~:text=Windstorms%20are%20amongst%20the%20most,annual%20losses%20in%20the%20EU.&amp;text=As%20a%20consequence%2C%20it%20is,rise%20due%20to%20climate%20change." xr:uid="{84766123-8B9C-40D7-9092-EE32EC59F2D3}"/>
-    <hyperlink ref="E97" r:id="rId74" xr:uid="{EE1C6824-4127-49BF-856B-54D15A26EEC3}"/>
+    <hyperlink ref="E68" r:id="rId60" xr:uid="{EE454482-8FED-4527-B986-77CD9C1F36C3}"/>
+    <hyperlink ref="E70" r:id="rId61" xr:uid="{4674AB5A-30F3-45D8-A76E-5D2DA2947D26}"/>
+    <hyperlink ref="E72" r:id="rId62" xr:uid="{6D1483F5-F282-415F-9759-DD789E670422}"/>
+    <hyperlink ref="E73" r:id="rId63" xr:uid="{7D4750D7-9B5F-418F-A8E0-1130FCCD84BF}"/>
+    <hyperlink ref="E79" r:id="rId64" xr:uid="{4DB7F4FC-198A-4F7C-99B5-E7956C26D0B4}"/>
+    <hyperlink ref="E82" r:id="rId65" xr:uid="{57799A75-4C8E-4C23-89A7-56A5834C31EE}"/>
+    <hyperlink ref="E83" r:id="rId66" xr:uid="{56C7BD61-7179-492F-B56F-8CB6DDCEF01A}"/>
+    <hyperlink ref="E87" r:id="rId67" xr:uid="{A62E077C-F1ED-4CCF-9B4D-44094647CCEB}"/>
+    <hyperlink ref="E89" r:id="rId68" xr:uid="{657B8500-1668-4027-AD3E-41D375A29A2F}"/>
+    <hyperlink ref="E90" r:id="rId69" xr:uid="{A51EE9E5-D6F9-4402-88D6-6938FEAAF425}"/>
+    <hyperlink ref="E94" r:id="rId70" xr:uid="{DAADEE44-3705-4408-AE31-5114CF9789AE}"/>
+    <hyperlink ref="E95" r:id="rId71" xr:uid="{2652C579-F57A-4A18-99E0-0CCE2D98D1BE}"/>
+    <hyperlink ref="E97" r:id="rId72" xr:uid="{F6E106D7-51E3-4796-8BCC-F62B4665CA66}"/>
+    <hyperlink ref="E96" r:id="rId73" location=":~:text=Windstorms%20are%20amongst%20the%20most,annual%20losses%20in%20the%20EU.&amp;text=As%20a%20consequence%2C%20it%20is,rise%20due%20to%20climate%20change." xr:uid="{84766123-8B9C-40D7-9092-EE32EC59F2D3}"/>
+    <hyperlink ref="E98" r:id="rId74" xr:uid="{EE1C6824-4127-49BF-856B-54D15A26EEC3}"/>
     <hyperlink ref="E27" r:id="rId75" xr:uid="{8772BA96-ED44-4481-A6D6-CAB4C1D2D36D}"/>
     <hyperlink ref="E100" r:id="rId76" xr:uid="{A8B1A50A-41B3-4028-8B6D-55BA1E74EF06}"/>
-    <hyperlink ref="E70" r:id="rId77" xr:uid="{7A6C35C0-065D-48C9-81B5-5BAC2E227370}"/>
+    <hyperlink ref="E71" r:id="rId77" xr:uid="{7A6C35C0-065D-48C9-81B5-5BAC2E227370}"/>
     <hyperlink ref="E106" r:id="rId78" xr:uid="{18FEDC5F-D897-4BD3-B5F5-B23D6192D5C7}"/>
     <hyperlink ref="E107" r:id="rId79" xr:uid="{188633F7-D468-4FF1-B629-6E1DEC4631EE}"/>
     <hyperlink ref="E108" r:id="rId80" xr:uid="{6FAF70A0-3FCF-454F-9682-BAB8A8C9D3E7}"/>
-    <hyperlink ref="E79" r:id="rId81" xr:uid="{D9A56F1D-2229-42A5-84AC-9DA4A78FF246}"/>
+    <hyperlink ref="E80" r:id="rId81" xr:uid="{D9A56F1D-2229-42A5-84AC-9DA4A78FF246}"/>
     <hyperlink ref="E42" r:id="rId82" xr:uid="{44C7D96C-57CD-4E32-B593-A7F8B9769E84}"/>
     <hyperlink ref="E54" r:id="rId83" xr:uid="{961F3F75-E073-4BB0-A98B-0BE784E6D0A8}"/>
     <hyperlink ref="E47" r:id="rId84" xr:uid="{6E06F162-E2CA-4ACE-B6F4-93389BC6A924}"/>
-    <hyperlink ref="E68" r:id="rId85" xr:uid="{A8F1B341-52CB-4E9C-A568-6E168B769DFA}"/>
+    <hyperlink ref="E69" r:id="rId85" xr:uid="{A8F1B341-52CB-4E9C-A568-6E168B769DFA}"/>
     <hyperlink ref="E40" r:id="rId86" xr:uid="{E6DCFA10-C08F-4A35-8D37-1141212EE65A}"/>
-    <hyperlink ref="E66" r:id="rId87" xr:uid="{1A7CB5D0-1D40-4507-A155-8D2A54EB5C0D}"/>
+    <hyperlink ref="E67" r:id="rId87" xr:uid="{1A7CB5D0-1D40-4507-A155-8D2A54EB5C0D}"/>
     <hyperlink ref="E50" r:id="rId88" xr:uid="{88DFAFA3-C726-468A-934C-491527C128D6}"/>
     <hyperlink ref="E48" r:id="rId89" xr:uid="{F591CC07-7435-4E15-9D93-39528ACCE89B}"/>
-    <hyperlink ref="E75" r:id="rId90" xr:uid="{ED87634C-0B58-4EAF-BEDB-2A48A969155C}"/>
+    <hyperlink ref="E76" r:id="rId90" xr:uid="{ED87634C-0B58-4EAF-BEDB-2A48A969155C}"/>
     <hyperlink ref="E105" r:id="rId91" xr:uid="{C77ED42E-2BAE-4561-B014-7D5CCCD7300B}"/>
     <hyperlink ref="E52" r:id="rId92" xr:uid="{AE60E41F-78E6-4C0B-99CC-9B9F011A14D2}"/>
     <hyperlink ref="E22" r:id="rId93" xr:uid="{D2CDFB65-960D-4324-9309-D75DB0AE6DE1}"/>
     <hyperlink ref="E32" r:id="rId94" xr:uid="{78010408-7D00-4480-9D3C-B780BB49E81D}"/>
     <hyperlink ref="E8" r:id="rId95" xr:uid="{2220BCD0-A5B0-4A1D-AA6D-A1D41EBDE3CE}"/>
     <hyperlink ref="E102" r:id="rId96" xr:uid="{3338E87A-5ECB-4F9B-ACE2-2EC0716ABFED}"/>
-    <hyperlink ref="E80" r:id="rId97" xr:uid="{C18AFA26-2EB1-499D-B2B4-72BB9C037E10}"/>
+    <hyperlink ref="E81" r:id="rId97" xr:uid="{C18AFA26-2EB1-499D-B2B4-72BB9C037E10}"/>
     <hyperlink ref="E26" r:id="rId98" xr:uid="{7D25A591-E8A8-418A-A32D-CDEB86ABCE99}"/>
     <hyperlink ref="E28" r:id="rId99" xr:uid="{2582EDBD-D337-4487-BD2B-35A6BA106688}"/>
-    <hyperlink ref="E76" r:id="rId100" xr:uid="{93645E69-F230-4737-B909-AF6297441E90}"/>
+    <hyperlink ref="E77" r:id="rId100" xr:uid="{93645E69-F230-4737-B909-AF6297441E90}"/>
     <hyperlink ref="E57" r:id="rId101" xr:uid="{A4270E10-FA55-4CD6-89BD-993EB73F11ED}"/>
     <hyperlink ref="E33" r:id="rId102" xr:uid="{7C482A88-1330-4A10-AE85-2F21D5F0D01B}"/>
     <hyperlink ref="E103" r:id="rId103" xr:uid="{82E79761-A535-494D-98AA-10AEED4B01D5}"/>
     <hyperlink ref="E58" r:id="rId104" xr:uid="{74A01E59-FEDC-471C-A936-DCE757B765DE}"/>
-    <hyperlink ref="E77" r:id="rId105" xr:uid="{C16C0228-218F-4349-9E17-C55FCC0E4848}"/>
-    <hyperlink ref="E83" r:id="rId106" xr:uid="{16CF4C79-2C66-473B-8376-0E52D53979DE}"/>
-    <hyperlink ref="E99" r:id="rId107" xr:uid="{6B3A7836-3287-4B71-BAE9-EBE88E438E91}"/>
+    <hyperlink ref="E78" r:id="rId105" xr:uid="{C16C0228-218F-4349-9E17-C55FCC0E4848}"/>
+    <hyperlink ref="E84" r:id="rId106" xr:uid="{16CF4C79-2C66-473B-8376-0E52D53979DE}"/>
+    <hyperlink ref="E61" r:id="rId107" xr:uid="{6B3A7836-3287-4B71-BAE9-EBE88E438E91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId108"/>

</xml_diff>